<commit_message>
Commit on 17 Feb 2019
</commit_message>
<xml_diff>
--- a/Santoshs_KeywordFrameworkPOM/Resources/FrameworkDriverExcel/FrameworkDriverExcel.xlsx
+++ b/Santoshs_KeywordFrameworkPOM/Resources/FrameworkDriverExcel/FrameworkDriverExcel.xlsx
@@ -10,62 +10,30 @@
     <sheet name="TestCases" sheetId="2" r:id="rId1"/>
     <sheet name="TestData" sheetId="1" r:id="rId2"/>
     <sheet name="GlobalConfig" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
-  <si>
-    <t>Retirement</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>PreRetirement</t>
   </si>
   <si>
-    <t>Field1</t>
-  </si>
-  <si>
-    <t>Field2</t>
-  </si>
-  <si>
-    <t>Field3</t>
-  </si>
-  <si>
-    <t>Field4</t>
-  </si>
-  <si>
-    <t>Field5</t>
-  </si>
-  <si>
-    <t>Very Conservative</t>
-  </si>
-  <si>
-    <t>Investor Profile</t>
-  </si>
-  <si>
-    <t>ROI</t>
-  </si>
-  <si>
     <t>TC#</t>
   </si>
   <si>
     <t>TC1</t>
   </si>
   <si>
-    <t>UI Section</t>
-  </si>
-  <si>
     <t>Execute</t>
   </si>
   <si>
     <t>Y</t>
   </si>
   <si>
-    <t>User Profile URL</t>
-  </si>
-  <si>
     <t>Keyword1</t>
   </si>
   <si>
@@ -94,6 +62,18 @@
   </si>
   <si>
     <t>ApplicationUrl</t>
+  </si>
+  <si>
+    <t>TC1_MercurySite|CloseBrowser</t>
+  </si>
+  <si>
+    <t>Keyword2</t>
+  </si>
+  <si>
+    <t>Mercury</t>
+  </si>
+  <si>
+    <t>mercury</t>
   </si>
 </sst>
 </file>
@@ -172,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -187,9 +167,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -198,9 +175,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -524,40 +498,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F9:F10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="11"/>
+    <col min="1" max="1" width="4.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="13" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>23</v>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -568,10 +549,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,132 +560,72 @@
     <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="8" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="8" t="s">
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="6">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2">
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="2">
-        <v>3</v>
-      </c>
-      <c r="I2" s="2">
-        <v>4</v>
-      </c>
-      <c r="J2" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="6">
-        <v>121</v>
-      </c>
-      <c r="E3" s="1">
-        <v>200</v>
-      </c>
-      <c r="F3" s="2">
-        <v>565</v>
-      </c>
-      <c r="G3" s="2">
-        <v>434</v>
-      </c>
-      <c r="H3" s="2">
-        <v>777</v>
-      </c>
-      <c r="I3" s="2">
-        <v>22323</v>
-      </c>
-      <c r="J3" s="2">
-        <v>4541312</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="6">
-        <v>12</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2">
-        <v>2</v>
-      </c>
-      <c r="H4" s="2">
-        <v>3</v>
-      </c>
-      <c r="I4" s="2">
-        <v>4</v>
-      </c>
-      <c r="J4" s="2">
-        <v>5</v>
+      <c r="C6" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -723,33 +644,51 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.140625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" style="10" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="17.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>21</v>
+      <c r="A1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>22</v>
+      <c r="A2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added TestNG Reporter a custom listenr class implementing ITestListers class
</commit_message>
<xml_diff>
--- a/Santoshs_KeywordFrameworkPOM/Resources/FrameworkDriverExcel/FrameworkDriverExcel.xlsx
+++ b/Santoshs_KeywordFrameworkPOM/Resources/FrameworkDriverExcel/FrameworkDriverExcel.xlsx
@@ -17,10 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
-  <si>
-    <t>PreRetirement</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>TC#</t>
   </si>
@@ -37,9 +34,6 @@
     <t>Keyword1</t>
   </si>
   <si>
-    <t>ConservativeEEEE</t>
-  </si>
-  <si>
     <t>ChromeWebDriver</t>
   </si>
   <si>
@@ -74,13 +68,16 @@
   </si>
   <si>
     <t>mercury</t>
+  </si>
+  <si>
+    <t>santosh.pandhare@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +97,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -149,10 +154,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -192,8 +198,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -498,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,30 +525,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -549,88 +573,58 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -653,24 +647,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -688,7 +682,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit Latest on 29 April 2019
</commit_message>
<xml_diff>
--- a/Santoshs_KeywordFrameworkPOM/Resources/FrameworkDriverExcel/FrameworkDriverExcel.xlsx
+++ b/Santoshs_KeywordFrameworkPOM/Resources/FrameworkDriverExcel/FrameworkDriverExcel.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
   <si>
     <t>TC#</t>
   </si>
@@ -511,7 +511,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,10 +573,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,6 +616,39 @@
         <v>17</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -676,7 +709,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>